<commit_message>
updated Ablaufplan and Antworten to 23.01.18
</commit_message>
<xml_diff>
--- a/aufgabe07/Ablaufplan.xlsx
+++ b/aufgabe07/Ablaufplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t xml:space="preserve">t</t>
   </si>
@@ -33,6 +33,48 @@
   </si>
   <si>
     <t xml:space="preserve">T3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3+R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2+R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(T4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(T5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(T6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIER DEADLOCK!</t>
   </si>
 </sst>
 </file>
@@ -47,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -64,7 +107,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,8 +126,32 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC00"/>
+        <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCCC"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00CC"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -106,6 +173,22 @@
       <right/>
       <top/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -134,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,7 +238,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,7 +279,7 @@
       <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFCC00CC"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
@@ -202,7 +305,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FF00CCCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -238,8 +341,8 @@
   </sheetPr>
   <dimension ref="A1:D202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S18" activeCellId="0" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1370,10 +1473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D252"/>
+  <dimension ref="A1:J252"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1386,13 +1489,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,253 +1510,287 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="E4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="1"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="1"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="2"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
+      <c r="E13" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="E22" s="5"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="7"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="7"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="C25" s="8"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="H30" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="H42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1666,37 +1806,33 @@
       <c r="A46" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -1717,45 +1853,47 @@
       <c r="A55" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="C55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="C56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="C57" s="1"/>
+      <c r="C57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="C58" s="1"/>
+      <c r="C58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>57</v>
       </c>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="C61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -1776,37 +1914,33 @@
       <c r="A66" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B69" s="2"/>
+      <c r="B69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -1882,37 +2016,33 @@
       <c r="A86" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="B86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="B87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="B88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="B89" s="2"/>
+      <c r="B89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>89</v>
       </c>
-      <c r="B91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -1983,81 +2113,89 @@
       <c r="A105" s="0" t="n">
         <v>103</v>
       </c>
-      <c r="C105" s="3"/>
+      <c r="D105" s="10"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
         <v>104</v>
       </c>
-      <c r="B106" s="3"/>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
         <v>105</v>
       </c>
-      <c r="B107" s="1"/>
+      <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
         <v>106</v>
       </c>
-      <c r="B108" s="1"/>
+      <c r="C108" s="2"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="B109" s="2"/>
+      <c r="B109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
         <v>108</v>
       </c>
-      <c r="B110" s="1"/>
+      <c r="C110" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
         <v>109</v>
       </c>
-      <c r="B111" s="1"/>
+      <c r="D111" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="C112" s="1"/>
+      <c r="D112" s="6"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
         <v>111</v>
       </c>
-      <c r="C113" s="1"/>
+      <c r="D113" s="7"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
         <v>112</v>
       </c>
-      <c r="C114" s="1"/>
+      <c r="D114" s="7"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
         <v>113</v>
       </c>
+      <c r="C115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
         <v>114</v>
       </c>
+      <c r="C116" s="8"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <v>115</v>
       </c>
+      <c r="C117" s="2"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <v>116</v>
       </c>
+      <c r="B118" s="2"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
@@ -2098,37 +2236,33 @@
       <c r="A126" s="0" t="n">
         <v>124</v>
       </c>
-      <c r="B126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="B127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="B128" s="1"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
         <v>127</v>
       </c>
-      <c r="B129" s="2"/>
+      <c r="B129" s="9"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
         <v>128</v>
       </c>
-      <c r="B130" s="1"/>
+      <c r="B130" s="2"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
         <v>129</v>
       </c>
-      <c r="B131" s="1"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
@@ -2204,37 +2338,33 @@
       <c r="A146" s="0" t="n">
         <v>144</v>
       </c>
-      <c r="B146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="B147" s="1"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
         <v>146</v>
       </c>
-      <c r="B148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B149" s="9"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
         <v>148</v>
       </c>
-      <c r="B150" s="1"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
         <v>149</v>
       </c>
-      <c r="B151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
@@ -2255,45 +2385,47 @@
       <c r="A155" s="0" t="n">
         <v>153</v>
       </c>
-      <c r="C155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
         <v>154</v>
       </c>
-      <c r="C156" s="1"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
         <v>155</v>
       </c>
-      <c r="C157" s="1"/>
+      <c r="C157" s="9"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
         <v>156</v>
       </c>
-      <c r="C158" s="1"/>
+      <c r="C158" s="2"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
         <v>157</v>
       </c>
+      <c r="C159" s="2"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
         <v>158</v>
       </c>
+      <c r="C160" s="8"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
         <v>159</v>
       </c>
+      <c r="C161" s="8"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="C162" s="2"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
@@ -2314,37 +2446,33 @@
       <c r="A166" s="0" t="n">
         <v>164</v>
       </c>
-      <c r="B166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="B167" s="1"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
         <v>166</v>
       </c>
-      <c r="B168" s="1"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
         <v>167</v>
       </c>
-      <c r="B169" s="2"/>
+      <c r="B169" s="9"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
         <v>168</v>
       </c>
-      <c r="B170" s="1"/>
+      <c r="B170" s="2"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
         <v>169</v>
       </c>
-      <c r="B171" s="1"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
@@ -2420,37 +2548,33 @@
       <c r="A186" s="0" t="n">
         <v>184</v>
       </c>
-      <c r="B186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="B187" s="1"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
         <v>186</v>
       </c>
-      <c r="B188" s="1"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
         <v>187</v>
       </c>
-      <c r="B189" s="2"/>
+      <c r="B189" s="9"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
         <v>188</v>
       </c>
-      <c r="B190" s="1"/>
+      <c r="B190" s="2"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="B191" s="1"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="n">
@@ -2509,6 +2633,7 @@
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
+      <c r="E202" s="4"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
@@ -2763,7 +2888,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
updated Ablaufplan and Antworten to final version
</commit_message>
<xml_diff>
--- a/aufgabe07/Ablaufplan.xlsx
+++ b/aufgabe07/Ablaufplan.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="A2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="A3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t xml:space="preserve">t</t>
   </si>
@@ -76,6 +77,33 @@
   <si>
     <t xml:space="preserve">HIER DEADLOCK!</t>
   </si>
+  <si>
+    <t xml:space="preserve">T8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Π = P(T8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(T8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5+R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Π = Prioritaet des hoechsten Tasks, der die Resource braucht</t>
+  </si>
 </sst>
 </file>
 
@@ -84,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,6 +133,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -217,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -259,6 +293,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,7 +383,7 @@
   </sheetPr>
   <dimension ref="A1:D202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S18" activeCellId="0" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -1475,8 +1517,8 @@
   </sheetPr>
   <dimension ref="A1:J252"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2892,4 +2934,1195 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I202"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="G9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" s="10"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="C60" s="10"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" s="10"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" s="8"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" s="10"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" s="8"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" s="10"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" s="2"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" s="8"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" s="2"/>
+      <c r="C110" s="12"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="C118" s="1"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="C120" s="1"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" s="10"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" s="8"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" s="10"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" s="8"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="n">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="n">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="n">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="C160" s="10"/>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" s="10"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" s="2"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" s="8"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" s="2"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" s="10"/>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" s="2"/>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" s="2"/>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" s="2"/>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" s="8"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" s="2"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="n">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" s="4"/>
+      <c r="C202" s="4"/>
+      <c r="D202" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>